<commit_message>
add new bug reports
add new bug reports
</commit_message>
<xml_diff>
--- a/Bug reports/Bug reports_main page.xlsx
+++ b/Bug reports/Bug reports_main page.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC9439E-FAA6-462A-B050-46B8474421D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78CC4FDC-4CC8-4106-A4B5-95C85E49F38B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="93">
   <si>
     <t>ID</t>
   </si>
@@ -44,12 +44,6 @@
   </si>
   <si>
     <t>Приложения</t>
-  </si>
-  <si>
-    <t>Низкий</t>
-  </si>
-  <si>
-    <t>Средний</t>
   </si>
   <si>
     <t>Windows 10 Pro, Yandex Browser
@@ -87,9 +81,6 @@
   </si>
   <si>
     <t>На главной странице при нажатии на кнопку "Войти"  открывается форма авторизации пользователя</t>
-  </si>
-  <si>
-    <t>Приоритет</t>
   </si>
   <si>
     <t>https://drive.google.com/file/d/1kiKYcbDsermXsGdnRsEM-SzCauA6798T/view?usp=sharingм</t>
@@ -262,12 +253,180 @@
   <si>
     <t>На главной странице домена yandex.uz под поисковой строкой нет баннера: "Новости переехали на dzen.ru"</t>
   </si>
+  <si>
+    <t>На главной странице при входе в приложение Почта открывается почтовый ящик, отличный от макета</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Запустить браузер 
+2. Запустить приложение Почта из боковой панели
+</t>
+  </si>
+  <si>
+    <t>1. Браузер запускается
+2. Приложение запускается в отдельном окне. В окне приложения баннер "Удобная Яндекс Почта с защитой от спама"</t>
+  </si>
+  <si>
+    <t>1. Браузер запускается
+2. Приложение запускается в отдельном окне. В окне приложения открывается почтовый ящик (см. скриншот)</t>
+  </si>
+  <si>
+    <t>Windows 10 Pro, Yandex Browser
+версия 23.1.5.708 (64-bit)</t>
+  </si>
+  <si>
+    <t>Minor</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1fneDgrABAQUSfMS9OjSG0L4710pnYPFr/view?usp=sharing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">На главной странице при входе в список приложений в списке Общение нет приложения ВКонтакте
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Запустить браузер 
+2. Нажать на кнопку «+» в боковой панели
+</t>
+  </si>
+  <si>
+    <t>1. Браузер запускается
+2. Появляется баллун</t>
+  </si>
+  <si>
+    <t>1. Браузер запускается 
+2. Появляется баллун без значка приложения Вконтакте в списке Общение (см. скриншот)</t>
+  </si>
+  <si>
+    <t>Major</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1ojX03jdrTF-qs30imyNsGbSeiuW9lVDp/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>При добавлении сайта pikabu.ru в меню добавления приложений появляется одна подсказка вместо двух</t>
+  </si>
+  <si>
+    <t>1. Запустить браузер 
+2. Нажать на кнопку «+» в боковой панели</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Нажать на кнопку «Добавить сайт как приложение»
+2. Ввести в строку pikabu.ru
+</t>
+  </si>
+  <si>
+    <t>1. Появляется меню добавления приложения
+2. Появляются 2 подсказки</t>
+  </si>
+  <si>
+    <t>1. Появляется меню добавления приложения
+2. Появляется одна подсказка (см. скриншот)</t>
+  </si>
+  <si>
+    <t>Trivial</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1JbUREOi8EFOlCHcMgGR1_9Czh_ncgCj9/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>При открытии новых страниц приложения pikabu.ru открытие страницы Курсы происходит внутри основного окна браузера</t>
+  </si>
+  <si>
+    <t>1. Запустить браузер 
+2. Нажать на кнопку «+» в боковой панели
+3. Нажать на кнопку «Добавить сайт как приложение»
+4.  Ввести в строку pikabu.ru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Выбрать первый вариант подсказки и кликнуть на него мышью
+2. Кликнуть на иконку приложения в боковой панели
+3. Прокликать по всем ссылкам в шапке сайта </t>
+  </si>
+  <si>
+    <t>1. Приложение устанавливается: в боковой панели появляется его иконка
+2. Приложение запустилось в отдельном окне
+3. Открытие новых страниц происходит внутри окна приложения, а не внутри основного окна браузера</t>
+  </si>
+  <si>
+    <t>1. Приложение устанавливается: в боковой панели появляется его иконка
+2. Приложение запустилось в отдельном окне
+3. Открытие страницы Курсы происходит внутри основного окна браузера</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/12pD_ocbs4GD5fOk1xUDS6FAkKqykESpi/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>При открытии сайта https://vk.com/  из боковой панели браузера приложение запускается на светлом фоне</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Запустить браузер
+2. В настройках браузера, в разделе Интерфейс, выбрать тему под названием «Прозрачная» 
+3. Перейти на сайт https://vk.com/ 
+4. Нажать на кнопку "Установить приложение" в адресной строке браузера
+5. Выбрать пункт «Всплывающее окно»
+6. Кликнуть по иконке "Вконтакте" в боковой панели
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Браузер запускается
+2. Тема применилась
+3. Сайт загружается
+4. Появляется баллун с выбором режима установки в отдельном окне, во всплывающем окне, в закрепленном окне
+5.Иконка приложения вылетела из адресной строки и прилетела в боковую панель
+6. Приложение запускается в виде всплывающего окна на темном фоне с темной боковой панелью
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Браузер запускается
+2. Тема применилась
+3. Сайт загружается
+4. Появляется баллун с выбором режима установки в отдельном окне, во всплывающем окне, в закрепленном окне
+5.Иконка приложения вылетела из адресной строки и прилетела в боковую панель
+6.  Приложение запускается в виде всплывающего окна на светлом фоне со светлой боковой панелью (см. скриншот)
+</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1p7zeXDJoVOR3xY3of5X_fx0ua-KpwIRS/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>BR-8</t>
+  </si>
+  <si>
+    <t>BR-9</t>
+  </si>
+  <si>
+    <t>BR-10</t>
+  </si>
+  <si>
+    <t>BR-11</t>
+  </si>
+  <si>
+    <t>BR-12</t>
+  </si>
+  <si>
+    <t>BR-13</t>
+  </si>
+  <si>
+    <t>BR-14</t>
+  </si>
+  <si>
+    <t>BR-15</t>
+  </si>
+  <si>
+    <t>BR-16</t>
+  </si>
+  <si>
+    <t>BR-17</t>
+  </si>
+  <si>
+    <t>Серьезность</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -308,6 +467,15 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -323,7 +491,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -444,12 +612,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -500,9 +683,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -539,10 +719,28 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -758,16 +956,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" customWidth="1"/>
+    <col min="1" max="1" width="6.21875" customWidth="1"/>
     <col min="2" max="2" width="23.5546875" customWidth="1"/>
     <col min="3" max="3" width="18.21875" customWidth="1"/>
     <col min="4" max="4" width="27.109375" customWidth="1"/>
@@ -800,203 +998,481 @@
         <v>1</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
-        <v>14</v>
+      <c r="A2" s="22" t="s">
+        <v>12</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="5" t="s">
+    </row>
+    <row r="3" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
-        <v>15</v>
-      </c>
       <c r="B3" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="8" t="s">
+    </row>
+    <row r="4" spans="1:9" ht="245.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="245.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="H4" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="8" t="s">
+    </row>
+    <row r="5" spans="1:9" s="12" customFormat="1" ht="151.80000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="11" t="s">
+      <c r="E5" s="20" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" s="12" customFormat="1" ht="151.80000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="F5" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="G5" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="99.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="17" t="s">
+      <c r="D6" s="14" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="99.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="E6" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="14" t="s">
+      <c r="F6" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="15" t="s">
+      <c r="G6" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I6" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="14" t="s">
+    </row>
+    <row r="7" spans="1:9" ht="200.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" s="19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="200.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+      <c r="B7" s="14" t="s">
         <v>40</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>43</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="152.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="21"/>
+      <c r="D8" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="15" t="s">
+      <c r="G8" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I8" s="29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="G7" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I7" s="19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="152.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="29" t="s">
+      <c r="E9" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="I8" s="30" t="s">
-        <v>48</v>
+      <c r="F9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="70.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="I10" s="30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="73.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" s="33" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="138.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="I12" s="34" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="192.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I13" s="35" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="I15" s="30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="76.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I16" s="33" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="141.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="I17" s="34" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="192.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I18" s="35" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1009,8 +1485,10 @@
     <hyperlink ref="I6" r:id="rId5" xr:uid="{2F96BCF6-4C0B-4C93-A619-6B574A2260E4}"/>
     <hyperlink ref="I7" r:id="rId6" xr:uid="{CA93259C-0B57-473D-BDBA-54BCD62FBB8C}"/>
     <hyperlink ref="I8" r:id="rId7" xr:uid="{6BB6758C-9BC3-4425-91DC-98A3BA2A35BE}"/>
+    <hyperlink ref="I9" r:id="rId8" display="https://drive.google.com/file/d/1BwrN4_tOs8A_uU1aASaASy-O8UioLUrv/view?usp=sharing" xr:uid="{03371A6D-6FB6-4368-A6EC-09410D94D1B7}"/>
+    <hyperlink ref="I14" r:id="rId9" display="https://drive.google.com/file/d/1BwrN4_tOs8A_uU1aASaASy-O8UioLUrv/view?usp=sharing" xr:uid="{517EF955-8834-404D-BD30-8F36F6E1DA0F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>